<commit_message>
0.3.22 - Improved cadet excel import logic.
</commit_message>
<xml_diff>
--- a/keel_cadet_import_template.xlsx
+++ b/keel_cadet_import_template.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Keel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C9DA79-4E06-4B1C-86B9-4EB8AFD19DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{869558DA-B6C0-4E20-B880-5519AE8D48DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadets" sheetId="1" r:id="rId1"/>
+    <sheet name="_meta" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="96">
+  <si>
+    <t>full_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>trainee_type</t>
+  </si>
   <si>
     <t>nationality</t>
   </si>
@@ -28,40 +33,277 @@
     <t>notes</t>
   </si>
   <si>
-    <t>Anuj Mengaji</t>
-  </si>
-  <si>
-    <t>anuj@example.com</t>
+    <t>rank_label</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>trb_applicable</t>
+  </si>
+  <si>
+    <t>Indian</t>
   </si>
   <si>
     <t>DECK_CADET</t>
   </si>
   <si>
-    <t>Indian</t>
-  </si>
-  <si>
-    <t>Onboarded via batch import</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>full_name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>trainee_type</t>
-  </si>
-  <si>
-    <t>rank_label</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>trb_applicable</t>
+    <t>ENGINE_CADET</t>
+  </si>
+  <si>
+    <t>ETO_CADET</t>
+  </si>
+  <si>
+    <t>DECK_RATING</t>
+  </si>
+  <si>
+    <t>ENGINE_RATING</t>
+  </si>
+  <si>
+    <t>Aarav Patel</t>
+  </si>
+  <si>
+    <t>aarav.patel@keel.test</t>
+  </si>
+  <si>
+    <t>Batch 2024</t>
+  </si>
+  <si>
+    <t>Deck Cadet</t>
+  </si>
+  <si>
+    <t>Cadet</t>
+  </si>
+  <si>
+    <t>Sofia Rossi</t>
+  </si>
+  <si>
+    <t>sofia.rossi@keel.test</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>Fast track</t>
+  </si>
+  <si>
+    <t>Engine Cadet</t>
+  </si>
+  <si>
+    <t>Wei Zhang</t>
+  </si>
+  <si>
+    <t>wei.zhang@keel.test</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>ETO Cadet</t>
+  </si>
+  <si>
+    <t>Liam O'Connor</t>
+  </si>
+  <si>
+    <t>liam.oconnor@keel.test</t>
+  </si>
+  <si>
+    <t>Irish</t>
+  </si>
+  <si>
+    <t>Experienced</t>
+  </si>
+  <si>
+    <t>Deck Rating</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Noah Müller</t>
+  </si>
+  <si>
+    <t>noah.muller@keel.test</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Engine Rating</t>
+  </si>
+  <si>
+    <t>Priya Sharma</t>
+  </si>
+  <si>
+    <t>priya.sharma@keel.test</t>
+  </si>
+  <si>
+    <t>Carlos Gomez</t>
+  </si>
+  <si>
+    <t>carlos.gomez@keel.test</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Yuki Tanaka</t>
+  </si>
+  <si>
+    <t>yuki.tanaka@keel.test</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>Olav Jensen</t>
+  </si>
+  <si>
+    <t>olav.jensen@keel.test</t>
+  </si>
+  <si>
+    <t>Norwegian</t>
+  </si>
+  <si>
+    <t>Lucas Silva</t>
+  </si>
+  <si>
+    <t>lucas.silva@keel.test</t>
+  </si>
+  <si>
+    <t>Brazilian</t>
+  </si>
+  <si>
+    <t>Emma Wilson</t>
+  </si>
+  <si>
+    <t>emma.wilson@keel.test</t>
+  </si>
+  <si>
+    <t>British</t>
+  </si>
+  <si>
+    <t>Ahmed Hassan</t>
+  </si>
+  <si>
+    <t>ahmed.hassan@keel.test</t>
+  </si>
+  <si>
+    <t>Egyptian</t>
+  </si>
+  <si>
+    <t>Ivan Petrov</t>
+  </si>
+  <si>
+    <t>ivan.petrov@keel.test</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Lars Nielsen</t>
+  </si>
+  <si>
+    <t>lars.nielsen@keel.test</t>
+  </si>
+  <si>
+    <t>Danish</t>
+  </si>
+  <si>
+    <t>Maria Santos</t>
+  </si>
+  <si>
+    <t>maria.santos@keel.test</t>
+  </si>
+  <si>
+    <t>Filipino</t>
+  </si>
+  <si>
+    <t>Chen Wei</t>
+  </si>
+  <si>
+    <t>chen.wei@keel.test</t>
+  </si>
+  <si>
+    <t>Juan Martinez</t>
+  </si>
+  <si>
+    <t>juan.martinez@keel.test</t>
+  </si>
+  <si>
+    <t>Mexican</t>
+  </si>
+  <si>
+    <t>Sarah Johnson</t>
+  </si>
+  <si>
+    <t>sarah.johnson@keel.test</t>
+  </si>
+  <si>
+    <t>American</t>
+  </si>
+  <si>
+    <t>Kim Min-jun</t>
+  </si>
+  <si>
+    <t>kim.minjun@keel.test</t>
+  </si>
+  <si>
+    <t>South Korean</t>
+  </si>
+  <si>
+    <t>Ali Reza</t>
+  </si>
+  <si>
+    <t>ali.reza@keel.test</t>
+  </si>
+  <si>
+    <t>Iranian</t>
+  </si>
+  <si>
+    <t>Thomas Dubois</t>
+  </si>
+  <si>
+    <t>thomas.dubois@keel.test</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Ana Kowalska</t>
+  </si>
+  <si>
+    <t>ana.kowalska@keel.test</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>Gabriel Costa</t>
+  </si>
+  <si>
+    <t>gabriel.costa@keel.test</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>Hina Khan</t>
+  </si>
+  <si>
+    <t>hina.khan@keel.test</t>
+  </si>
+  <si>
+    <t>Pakistani</t>
+  </si>
+  <si>
+    <t>James Cook</t>
+  </si>
+  <si>
+    <t>james.cook@keel.test</t>
+  </si>
+  <si>
+    <t>Australian</t>
   </si>
 </sst>
 </file>
@@ -70,7 +312,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -104,7 +346,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -438,76 +680,686 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="18.875" customWidth="1"/>
-    <col min="6" max="6" width="37.875" customWidth="1"/>
-    <col min="7" max="7" width="35.875" customWidth="1"/>
-    <col min="8" max="8" width="41.875" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2:H2 D1:E1" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please select a valid Trainee Type from the dropdown." xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>_meta!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1000</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>